<commit_message>
Further development of Bz code, phases match but amplitude is still questionable.
</commit_message>
<xml_diff>
--- a/BrShift.xlsx
+++ b/BrShift.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/EDM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B170A1FA-A10B-FC41-83D6-3341A4010837}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF6DF19-045C-F742-8C10-E86C38184799}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="16040" xr2:uid="{85812D83-8DEC-B647-9A33-A6CE083631F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -96,8 +96,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B59DA7-83C3-B247-A41E-5F3E9BC3DE79}">
-  <dimension ref="C1:I6"/>
+  <dimension ref="C1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -424,7 +427,7 @@
     <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D1" t="s">
         <v>3</v>
       </c>
@@ -432,7 +435,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D2">
         <v>-0.74199999999999999</v>
       </c>
@@ -440,7 +443,7 @@
         <v>0.47499999999999998</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -462,8 +465,11 @@
       <c r="I4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C5">
         <v>0.12</v>
       </c>
@@ -489,9 +495,16 @@
         <f>SQRT($E$2^2+G5^2)</f>
         <v>0.47499999999999998</v>
       </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C6">
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <f>SQRT(L4^2+L5^2)</f>
+        <v>2.2360679774997898</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C6" s="1">
         <f>74.7989-74.7089</f>
         <v>9.0000000000003411E-2</v>
       </c>
@@ -517,6 +530,35 @@
       <c r="I6">
         <f>SQRT($E$2^2+G6^2)</f>
         <v>0.47628030928928378</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <f>SQRT(M5^2+L6^2)</f>
+        <v>3.7416573867739413</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <f>SQRT(M6^2+L7^2)</f>
+        <v>5.4772255750516612</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="L8">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <f>SQRT(M7^2+L8^2)</f>
+        <v>7.416198487095663</v>
+      </c>
+      <c r="N8">
+        <f>SQRT(L4^2+L5^2+L6^2+L8^2+L7^2)</f>
+        <v>7.416198487095663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>